<commit_message>
add a column with Continent definition of EU27 to additional_information.xlsx
</commit_message>
<xml_diff>
--- a/Input_Data/default_scenario/02_Additional_Information/additional_information.xlsx
+++ b/Input_Data/default_scenario/02_Additional_Information/additional_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honkomp\PycharmProjects\oop_pytigfpm\GFPMpt\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_Projekte\P_TiMBA_AddInfo\TiMBA_Additional_Information\Input_Data\default_scenario\02_Additional_Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19041A4E-7229-4AC9-B208-4A0BC71E8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B67B3CA5-A038-4DD4-81BD-EDB8A03F3E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="276" yWindow="3288" windowWidth="21960" windowHeight="11880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="-15510" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Country" sheetId="1" r:id="rId1"/>
@@ -27,11 +27,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Country!$A$1:$J$181</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="676">
   <si>
     <t>Country</t>
   </si>
@@ -1797,60 +1808,18 @@
     <t>ContinentNew</t>
   </si>
   <si>
-    <t>xnf</t>
-  </si>
-  <si>
     <t>MENA</t>
   </si>
   <si>
-    <t>xac</t>
-  </si>
-  <si>
     <t>SSA</t>
   </si>
   <si>
-    <t>ben</t>
-  </si>
-  <si>
-    <t>bfa</t>
-  </si>
-  <si>
-    <t>xec</t>
-  </si>
-  <si>
-    <t>xwf</t>
-  </si>
-  <si>
-    <t>xcf</t>
-  </si>
-  <si>
-    <t>civ</t>
-  </si>
-  <si>
-    <t>gin</t>
-  </si>
-  <si>
-    <t>xsc</t>
-  </si>
-  <si>
     <t>fra</t>
   </si>
   <si>
-    <t>rwa</t>
-  </si>
-  <si>
-    <t>tgo</t>
-  </si>
-  <si>
-    <t>xcb</t>
-  </si>
-  <si>
     <t>RestLatiAmer</t>
   </si>
   <si>
-    <t>xca</t>
-  </si>
-  <si>
     <t>can</t>
   </si>
   <si>
@@ -1863,21 +1832,9 @@
     <t>bra</t>
   </si>
   <si>
-    <t>xsm</t>
-  </si>
-  <si>
-    <t>ven</t>
-  </si>
-  <si>
-    <t>xsa</t>
-  </si>
-  <si>
     <t>RestAsia</t>
   </si>
   <si>
-    <t>xse</t>
-  </si>
-  <si>
     <t>chn</t>
   </si>
   <si>
@@ -1887,15 +1844,9 @@
     <t>ind</t>
   </si>
   <si>
-    <t>xws</t>
-  </si>
-  <si>
     <t>jpn</t>
   </si>
   <si>
-    <t>xea</t>
-  </si>
-  <si>
     <t>kor</t>
   </si>
   <si>
@@ -1905,15 +1856,9 @@
     <t>aus</t>
   </si>
   <si>
-    <t>xoc</t>
-  </si>
-  <si>
     <t>nzl</t>
   </si>
   <si>
-    <t>xer</t>
-  </si>
-  <si>
     <t>deu</t>
   </si>
   <si>
@@ -1926,21 +1871,12 @@
     <t>RestCIS</t>
   </si>
   <si>
-    <t>xee</t>
-  </si>
-  <si>
     <t>rus</t>
   </si>
   <si>
-    <t>xsu</t>
-  </si>
-  <si>
     <t>ukr</t>
   </si>
   <si>
-    <t>MagnetCou-Code</t>
-  </si>
-  <si>
     <t>MagnetRegion</t>
   </si>
   <si>
@@ -2125,6 +2061,15 @@
   </si>
   <si>
     <t>Sawnwood C</t>
+  </si>
+  <si>
+    <t>Rest of Europe</t>
+  </si>
+  <si>
+    <t>EU27</t>
+  </si>
+  <si>
+    <t>ContinentNew_v2</t>
   </si>
 </sst>
 </file>
@@ -2659,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K182"/>
+  <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,10 +2620,10 @@
     <col min="6" max="6" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="2"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2686,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>694</v>
+        <v>669</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2707,13 +2652,13 @@
         <v>587</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>635</v>
+        <v>675</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>636</v>
+        <v>611</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>685</v>
+        <v>660</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2741,14 +2686,14 @@
       <c r="H2" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
+        <v>550</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>589</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>693</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2776,14 +2721,14 @@
       <c r="H3" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>590</v>
+      <c r="I3" t="s">
+        <v>550</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2811,14 +2756,14 @@
       <c r="H4" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>592</v>
+      <c r="I4" t="s">
+        <v>550</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2846,14 +2791,14 @@
       <c r="H5" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>16</v>
+      <c r="I5" t="s">
+        <v>550</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2881,14 +2826,14 @@
       <c r="H6" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>593</v>
+      <c r="I6" t="s">
+        <v>550</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2916,14 +2861,14 @@
       <c r="H7" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>594</v>
+      <c r="I7" t="s">
+        <v>550</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2951,14 +2896,14 @@
       <c r="H8" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>25</v>
+      <c r="I8" t="s">
+        <v>550</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2986,14 +2931,14 @@
       <c r="H9" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>595</v>
+      <c r="I9" t="s">
+        <v>550</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3021,14 +2966,14 @@
       <c r="H10" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>596</v>
+      <c r="I10" t="s">
+        <v>550</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3056,14 +3001,14 @@
       <c r="H11" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>596</v>
+      <c r="I11" t="s">
+        <v>550</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3091,14 +3036,14 @@
       <c r="H12" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>596</v>
+      <c r="I12" t="s">
+        <v>550</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3126,14 +3071,14 @@
       <c r="H13" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>597</v>
+      <c r="I13" t="s">
+        <v>550</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3161,14 +3106,14 @@
       <c r="H14" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>594</v>
+      <c r="I14" t="s">
+        <v>550</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3196,14 +3141,14 @@
       <c r="H15" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>47</v>
+      <c r="I15" t="s">
+        <v>550</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>693</v>
+        <v>668</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3231,14 +3176,14 @@
       <c r="H16" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>596</v>
+      <c r="I16" t="s">
+        <v>550</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3266,14 +3211,14 @@
       <c r="H17" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>54</v>
+      <c r="I17" t="s">
+        <v>550</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3301,14 +3246,14 @@
       <c r="H18" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>596</v>
+      <c r="I18" t="s">
+        <v>550</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3336,14 +3281,14 @@
       <c r="H19" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>595</v>
+      <c r="I19" t="s">
+        <v>550</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3371,14 +3316,14 @@
       <c r="H20" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>63</v>
+      <c r="I20" t="s">
+        <v>550</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3406,14 +3351,14 @@
       <c r="H21" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>598</v>
+      <c r="I21" t="s">
+        <v>550</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3441,14 +3386,14 @@
       <c r="H22" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>595</v>
+      <c r="I22" t="s">
+        <v>550</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3476,14 +3421,14 @@
       <c r="H23" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>72</v>
+      <c r="I23" t="s">
+        <v>550</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,14 +3456,14 @@
       <c r="H24" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>599</v>
+      <c r="I24" t="s">
+        <v>550</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3546,14 +3491,14 @@
       <c r="H25" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>595</v>
+      <c r="I25" t="s">
+        <v>550</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3581,14 +3526,14 @@
       <c r="H26" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" t="s">
+        <v>550</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>589</v>
-      </c>
       <c r="K26" s="2" t="s">
-        <v>693</v>
+        <v>668</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3616,14 +3561,14 @@
       <c r="H27" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>85</v>
+      <c r="I27" t="s">
+        <v>550</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3651,14 +3596,14 @@
       <c r="H28" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>88</v>
+      <c r="I28" t="s">
+        <v>550</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3686,14 +3631,14 @@
       <c r="H29" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>595</v>
+      <c r="I29" t="s">
+        <v>550</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3721,14 +3666,14 @@
       <c r="H30" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>595</v>
+      <c r="I30" t="s">
+        <v>550</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3756,14 +3701,14 @@
       <c r="H31" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>97</v>
+      <c r="I31" t="s">
+        <v>550</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3791,14 +3736,14 @@
       <c r="H32" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>100</v>
+      <c r="I32" t="s">
+        <v>550</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>693</v>
+        <v>668</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3826,14 +3771,14 @@
       <c r="H33" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>103</v>
+      <c r="I33" t="s">
+        <v>550</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3861,14 +3806,14 @@
       <c r="H34" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>595</v>
+      <c r="I34" t="s">
+        <v>550</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3896,14 +3841,14 @@
       <c r="H35" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>109</v>
+      <c r="I35" t="s">
+        <v>550</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3923,7 +3868,7 @@
         <v>550</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>6</v>
@@ -3931,14 +3876,14 @@
       <c r="H36" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>600</v>
+      <c r="I36" t="s">
+        <v>550</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3966,14 +3911,14 @@
       <c r="H37" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>601</v>
+      <c r="I37" t="s">
+        <v>550</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4001,14 +3946,14 @@
       <c r="H38" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>596</v>
+      <c r="I38" t="s">
+        <v>550</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -4036,14 +3981,14 @@
       <c r="H39" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>121</v>
+      <c r="I39" t="s">
+        <v>550</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -4071,14 +4016,14 @@
       <c r="H40" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>595</v>
+      <c r="I40" t="s">
+        <v>550</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -4106,14 +4051,14 @@
       <c r="H41" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>594</v>
+      <c r="I41" t="s">
+        <v>550</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -4141,14 +4086,14 @@
       <c r="H42" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>130</v>
+      <c r="I42" t="s">
+        <v>550</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -4176,14 +4121,14 @@
       <c r="H43" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>594</v>
+      <c r="I43" t="s">
+        <v>550</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -4211,14 +4156,14 @@
       <c r="H44" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>599</v>
+      <c r="I44" t="s">
+        <v>550</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -4246,14 +4191,14 @@
       <c r="H45" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>139</v>
+      <c r="I45" t="s">
+        <v>550</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -4281,14 +4226,14 @@
       <c r="H46" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>602</v>
+      <c r="I46" t="s">
+        <v>550</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4316,14 +4261,14 @@
       <c r="H47" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>145</v>
+      <c r="I47" t="s">
+        <v>550</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>693</v>
+        <v>668</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4351,14 +4296,14 @@
       <c r="H48" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>148</v>
+      <c r="I48" t="s">
+        <v>550</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -4386,14 +4331,14 @@
       <c r="H49" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>590</v>
+      <c r="I49" t="s">
+        <v>550</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>691</v>
+        <v>666</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4421,14 +4366,14 @@
       <c r="H50" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>154</v>
+      <c r="I50" t="s">
+        <v>550</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -4456,14 +4401,14 @@
       <c r="H51" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>157</v>
+      <c r="I51" t="s">
+        <v>550</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -4491,14 +4436,14 @@
       <c r="H52" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>603</v>
+      <c r="I52" t="s">
+        <v>556</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -4526,14 +4471,14 @@
       <c r="H53" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>603</v>
+      <c r="I53" t="s">
+        <v>556</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -4561,14 +4506,14 @@
       <c r="H54" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>605</v>
+      <c r="I54" t="s">
+        <v>556</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -4596,11 +4541,11 @@
       <c r="H55" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>169</v>
+      <c r="I55" t="s">
+        <v>556</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>556</v>
@@ -4631,14 +4576,14 @@
       <c r="H56" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>603</v>
+      <c r="I56" t="s">
+        <v>556</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4666,14 +4611,14 @@
       <c r="H57" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>176</v>
+      <c r="I57" t="s">
+        <v>556</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4701,14 +4646,14 @@
       <c r="H58" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>603</v>
+      <c r="I58" t="s">
+        <v>556</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4736,14 +4681,14 @@
       <c r="H59" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>603</v>
+      <c r="I59" t="s">
+        <v>556</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4771,14 +4716,14 @@
       <c r="H60" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>603</v>
+      <c r="I60" t="s">
+        <v>556</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4806,14 +4751,14 @@
       <c r="H61" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>188</v>
+      <c r="I61" t="s">
+        <v>556</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -4841,14 +4786,14 @@
       <c r="H62" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>191</v>
+      <c r="I62" t="s">
+        <v>556</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -4876,14 +4821,14 @@
       <c r="H63" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I63" s="2" t="s">
-        <v>603</v>
+      <c r="I63" t="s">
+        <v>556</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -4911,14 +4856,14 @@
       <c r="H64" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I64" s="2" t="s">
-        <v>197</v>
+      <c r="I64" t="s">
+        <v>556</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -4946,14 +4891,14 @@
       <c r="H65" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I65" s="2" t="s">
-        <v>603</v>
+      <c r="I65" t="s">
+        <v>556</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -4973,7 +4918,7 @@
         <v>556</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>6</v>
@@ -4981,14 +4926,14 @@
       <c r="H66" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I66" s="2" t="s">
-        <v>600</v>
+      <c r="I66" t="s">
+        <v>556</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -5016,14 +4961,14 @@
       <c r="H67" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I67" s="2" t="s">
-        <v>206</v>
+      <c r="I67" t="s">
+        <v>556</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -5043,7 +4988,7 @@
         <v>556</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>6</v>
@@ -5051,14 +4996,14 @@
       <c r="H68" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I68" s="2" t="s">
-        <v>603</v>
+      <c r="I68" t="s">
+        <v>556</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -5086,14 +5031,14 @@
       <c r="H69" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I69" s="2" t="s">
-        <v>212</v>
+      <c r="I69" t="s">
+        <v>556</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -5121,14 +5066,14 @@
       <c r="H70" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I70" s="2" t="s">
-        <v>215</v>
+      <c r="I70" t="s">
+        <v>556</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -5156,14 +5101,14 @@
       <c r="H71" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I71" s="2" t="s">
-        <v>603</v>
+      <c r="I71" t="s">
+        <v>556</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -5191,14 +5136,14 @@
       <c r="H72" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>603</v>
+      <c r="I72" t="s">
+        <v>556</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -5226,11 +5171,11 @@
       <c r="H73" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I73" s="2" t="s">
-        <v>224</v>
+      <c r="I73" t="s">
+        <v>556</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>556</v>
@@ -5261,11 +5206,11 @@
       <c r="H74" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I74" s="2" t="s">
-        <v>228</v>
+      <c r="I74" t="s">
+        <v>551</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>551</v>
@@ -5296,11 +5241,11 @@
       <c r="H75" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I75" s="2" t="s">
-        <v>231</v>
+      <c r="I75" t="s">
+        <v>551</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>551</v>
@@ -5331,11 +5276,11 @@
       <c r="H76" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>234</v>
+      <c r="I76" t="s">
+        <v>551</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>551</v>
@@ -5366,11 +5311,11 @@
       <c r="H77" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I77" s="2" t="s">
-        <v>237</v>
+      <c r="I77" t="s">
+        <v>551</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>551</v>
@@ -5401,11 +5346,11 @@
       <c r="H78" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I78" s="2" t="s">
-        <v>240</v>
+      <c r="I78" t="s">
+        <v>551</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>551</v>
@@ -5436,11 +5381,11 @@
       <c r="H79" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I79" s="2" t="s">
-        <v>243</v>
+      <c r="I79" t="s">
+        <v>551</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>551</v>
@@ -5463,7 +5408,7 @@
         <v>551</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>6</v>
@@ -5471,11 +5416,11 @@
       <c r="H80" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I80" s="2" t="s">
-        <v>610</v>
+      <c r="I80" t="s">
+        <v>551</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>551</v>
@@ -5506,11 +5451,11 @@
       <c r="H81" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I81" s="2" t="s">
-        <v>610</v>
+      <c r="I81" t="s">
+        <v>551</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>551</v>
@@ -5541,11 +5486,11 @@
       <c r="H82" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I82" s="2" t="s">
-        <v>252</v>
+      <c r="I82" t="s">
+        <v>551</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>551</v>
@@ -5576,11 +5521,11 @@
       <c r="H83" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I83" s="2" t="s">
-        <v>255</v>
+      <c r="I83" t="s">
+        <v>551</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>551</v>
@@ -5611,11 +5556,11 @@
       <c r="H84" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I84" s="2" t="s">
-        <v>610</v>
+      <c r="I84" t="s">
+        <v>551</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>551</v>
@@ -5646,11 +5591,11 @@
       <c r="H85" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I85" s="2" t="s">
-        <v>261</v>
+      <c r="I85" t="s">
+        <v>551</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K85" s="2" t="s">
         <v>551</v>
@@ -5681,11 +5626,11 @@
       <c r="H86" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="I86" s="2" t="s">
-        <v>611</v>
+      <c r="I86" t="s">
+        <v>551</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>551</v>
@@ -5716,14 +5661,14 @@
       <c r="H87" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I87" s="2" t="s">
-        <v>612</v>
+      <c r="I87" t="s">
+        <v>552</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -5751,14 +5696,14 @@
       <c r="H88" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I88" s="2" t="s">
-        <v>270</v>
+      <c r="I88" t="s">
+        <v>552</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -5786,14 +5731,14 @@
       <c r="H89" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>273</v>
+      <c r="I89" t="s">
+        <v>552</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -5821,14 +5766,14 @@
       <c r="H90" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I90" s="2" t="s">
-        <v>612</v>
+      <c r="I90" t="s">
+        <v>552</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -5856,14 +5801,14 @@
       <c r="H91" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I91" s="2" t="s">
-        <v>614</v>
+      <c r="I91" t="s">
+        <v>552</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -5891,14 +5836,14 @@
       <c r="H92" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I92" s="2" t="s">
-        <v>282</v>
+      <c r="I92" t="s">
+        <v>552</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -5926,14 +5871,14 @@
       <c r="H93" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I93" s="2" t="s">
-        <v>285</v>
+      <c r="I93" t="s">
+        <v>552</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -5961,14 +5906,14 @@
       <c r="H94" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I94" s="2" t="s">
-        <v>288</v>
+      <c r="I94" t="s">
+        <v>552</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -5996,14 +5941,14 @@
       <c r="H95" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I95" s="2" t="s">
-        <v>612</v>
+      <c r="I95" t="s">
+        <v>552</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -6031,14 +5976,14 @@
       <c r="H96" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I96" s="2" t="s">
-        <v>294</v>
+      <c r="I96" t="s">
+        <v>552</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>617</v>
+        <v>599</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -6066,14 +6011,14 @@
       <c r="H97" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I97" s="2" t="s">
-        <v>297</v>
+      <c r="I97" t="s">
+        <v>552</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -6101,14 +6046,14 @@
       <c r="H98" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I98" s="2" t="s">
-        <v>300</v>
+      <c r="I98" t="s">
+        <v>552</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -6136,14 +6081,14 @@
       <c r="H99" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I99" s="2" t="s">
-        <v>618</v>
+      <c r="I99" t="s">
+        <v>552</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -6171,14 +6116,14 @@
       <c r="H100" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I100" s="2" t="s">
-        <v>306</v>
+      <c r="I100" t="s">
+        <v>552</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -6206,14 +6151,14 @@
       <c r="H101" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I101" s="2" t="s">
-        <v>309</v>
+      <c r="I101" t="s">
+        <v>552</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>619</v>
+        <v>600</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -6241,14 +6186,14 @@
       <c r="H102" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I102" s="2" t="s">
-        <v>618</v>
+      <c r="I102" t="s">
+        <v>552</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -6276,14 +6221,14 @@
       <c r="H103" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I103" s="2" t="s">
-        <v>620</v>
+      <c r="I103" t="s">
+        <v>552</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -6311,14 +6256,14 @@
       <c r="H104" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I104" s="2" t="s">
-        <v>318</v>
+      <c r="I104" t="s">
+        <v>552</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -6346,14 +6291,14 @@
       <c r="H105" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>321</v>
+      <c r="I105" t="s">
+        <v>552</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -6381,14 +6326,14 @@
       <c r="H106" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I106" s="2" t="s">
-        <v>324</v>
+      <c r="I106" t="s">
+        <v>552</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -6416,14 +6361,14 @@
       <c r="H107" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I107" s="2" t="s">
-        <v>618</v>
+      <c r="I107" t="s">
+        <v>552</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -6451,14 +6396,14 @@
       <c r="H108" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I108" s="2" t="s">
-        <v>614</v>
+      <c r="I108" t="s">
+        <v>552</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -6486,14 +6431,14 @@
       <c r="H109" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I109" s="2" t="s">
-        <v>333</v>
+      <c r="I109" t="s">
+        <v>552</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -6521,14 +6466,14 @@
       <c r="H110" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I110" s="2" t="s">
-        <v>336</v>
+      <c r="I110" t="s">
+        <v>552</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -6556,14 +6501,14 @@
       <c r="H111" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I111" s="2" t="s">
-        <v>614</v>
+      <c r="I111" t="s">
+        <v>552</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
@@ -6591,14 +6536,14 @@
       <c r="H112" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I112" s="2" t="s">
-        <v>342</v>
+      <c r="I112" t="s">
+        <v>552</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -6626,14 +6571,14 @@
       <c r="H113" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I113" s="2" t="s">
-        <v>345</v>
+      <c r="I113" t="s">
+        <v>552</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
@@ -6661,14 +6606,14 @@
       <c r="H114" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I114" s="2" t="s">
-        <v>348</v>
+      <c r="I114" t="s">
+        <v>552</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
@@ -6696,14 +6641,14 @@
       <c r="H115" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I115" s="2" t="s">
-        <v>351</v>
+      <c r="I115" t="s">
+        <v>552</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -6731,14 +6676,14 @@
       <c r="H116" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I116" s="2" t="s">
-        <v>354</v>
+      <c r="I116" t="s">
+        <v>552</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -6766,14 +6711,14 @@
       <c r="H117" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I117" s="2" t="s">
-        <v>357</v>
+      <c r="I117" t="s">
+        <v>552</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -6801,14 +6746,14 @@
       <c r="H118" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I118" s="2" t="s">
-        <v>360</v>
+      <c r="I118" t="s">
+        <v>552</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -6836,14 +6781,14 @@
       <c r="H119" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I119" s="2" t="s">
-        <v>363</v>
+      <c r="I119" t="s">
+        <v>552</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -6871,14 +6816,14 @@
       <c r="H120" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I120" s="2" t="s">
-        <v>618</v>
+      <c r="I120" t="s">
+        <v>552</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -6906,14 +6851,14 @@
       <c r="H121" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I121" s="2" t="s">
-        <v>369</v>
+      <c r="I121" t="s">
+        <v>552</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -6941,14 +6886,14 @@
       <c r="H122" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I122" s="2" t="s">
-        <v>372</v>
+      <c r="I122" t="s">
+        <v>552</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -6976,14 +6921,14 @@
       <c r="H123" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I123" s="2" t="s">
-        <v>375</v>
+      <c r="I123" t="s">
+        <v>552</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -7011,14 +6956,14 @@
       <c r="H124" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I124" s="2" t="s">
-        <v>378</v>
+      <c r="I124" t="s">
+        <v>552</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>689</v>
+        <v>664</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
@@ -7046,14 +6991,14 @@
       <c r="H125" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I125" s="2" t="s">
-        <v>618</v>
+      <c r="I125" t="s">
+        <v>552</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -7081,11 +7026,11 @@
       <c r="H126" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I126" s="2" t="s">
-        <v>384</v>
+      <c r="I126" t="s">
+        <v>553</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="K126" s="2" t="s">
         <v>553</v>
@@ -7108,7 +7053,7 @@
         <v>553</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="G127" s="3" t="s">
         <v>6</v>
@@ -7116,11 +7061,11 @@
       <c r="H127" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I127" s="2" t="s">
-        <v>624</v>
+      <c r="I127" t="s">
+        <v>553</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K127" s="2" t="s">
         <v>553</v>
@@ -7151,11 +7096,11 @@
       <c r="H128" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I128" s="2" t="s">
-        <v>624</v>
+      <c r="I128" t="s">
+        <v>553</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K128" s="2" t="s">
         <v>553</v>
@@ -7186,11 +7131,11 @@
       <c r="H129" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I129" s="2" t="s">
-        <v>624</v>
+      <c r="I129" t="s">
+        <v>553</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K129" s="2" t="s">
         <v>553</v>
@@ -7221,11 +7166,11 @@
       <c r="H130" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I130" s="2" t="s">
-        <v>624</v>
+      <c r="I130" t="s">
+        <v>553</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K130" s="2" t="s">
         <v>553</v>
@@ -7256,11 +7201,11 @@
       <c r="H131" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I131" s="2" t="s">
-        <v>399</v>
+      <c r="I131" t="s">
+        <v>553</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>625</v>
+        <v>604</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>553</v>
@@ -7291,11 +7236,11 @@
       <c r="H132" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I132" s="2" t="s">
-        <v>624</v>
+      <c r="I132" t="s">
+        <v>553</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K132" s="2" t="s">
         <v>553</v>
@@ -7326,11 +7271,11 @@
       <c r="H133" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I133" s="2" t="s">
-        <v>624</v>
+      <c r="I133" t="s">
+        <v>553</v>
       </c>
       <c r="J133" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K133" s="2" t="s">
         <v>553</v>
@@ -7361,11 +7306,11 @@
       <c r="H134" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I134" s="2" t="s">
-        <v>624</v>
+      <c r="I134" t="s">
+        <v>553</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K134" s="2" t="s">
         <v>553</v>
@@ -7396,11 +7341,11 @@
       <c r="H135" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I135" s="2" t="s">
-        <v>624</v>
+      <c r="I135" t="s">
+        <v>553</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K135" s="2" t="s">
         <v>553</v>
@@ -7431,11 +7376,11 @@
       <c r="H136" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I136" s="2" t="s">
-        <v>624</v>
+      <c r="I136" t="s">
+        <v>553</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K136" s="2" t="s">
         <v>553</v>
@@ -7466,11 +7411,11 @@
       <c r="H137" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I137" s="2" t="s">
-        <v>417</v>
+      <c r="I137" t="s">
+        <v>673</v>
       </c>
       <c r="J137" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K137" s="2" t="s">
         <v>554</v>
@@ -7501,11 +7446,11 @@
       <c r="H138" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I138" s="2" t="s">
-        <v>420</v>
+      <c r="I138" t="s">
+        <v>674</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K138" s="2" t="s">
         <v>554</v>
@@ -7536,11 +7481,11 @@
       <c r="H139" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I139" s="2" t="s">
-        <v>423</v>
+      <c r="I139" t="s">
+        <v>674</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K139" s="2" t="s">
         <v>554</v>
@@ -7571,11 +7516,11 @@
       <c r="H140" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I140" s="2" t="s">
-        <v>626</v>
+      <c r="I140" t="s">
+        <v>673</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>554</v>
@@ -7606,11 +7551,11 @@
       <c r="H141" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I141" s="2" t="s">
-        <v>429</v>
+      <c r="I141" t="s">
+        <v>674</v>
       </c>
       <c r="J141" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K141" s="2" t="s">
         <v>554</v>
@@ -7641,11 +7586,11 @@
       <c r="H142" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I142" s="2" t="s">
-        <v>432</v>
+      <c r="I142" t="s">
+        <v>674</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K142" s="2" t="s">
         <v>554</v>
@@ -7676,11 +7621,11 @@
       <c r="H143" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I143" s="2" t="s">
-        <v>435</v>
+      <c r="I143" t="s">
+        <v>674</v>
       </c>
       <c r="J143" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K143" s="2" t="s">
         <v>554</v>
@@ -7711,11 +7656,11 @@
       <c r="H144" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I144" s="2" t="s">
-        <v>438</v>
+      <c r="I144" t="s">
+        <v>674</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>554</v>
@@ -7746,11 +7691,11 @@
       <c r="H145" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I145" s="2" t="s">
-        <v>441</v>
+      <c r="I145" t="s">
+        <v>674</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>554</v>
@@ -7781,11 +7726,11 @@
       <c r="H146" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I146" s="2" t="s">
-        <v>444</v>
+      <c r="I146" t="s">
+        <v>674</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="K146" s="2" t="s">
         <v>554</v>
@@ -7816,11 +7761,11 @@
       <c r="H147" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I147" s="2" t="s">
-        <v>447</v>
+      <c r="I147" t="s">
+        <v>674</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>627</v>
+        <v>605</v>
       </c>
       <c r="K147" s="2" t="s">
         <v>554</v>
@@ -7851,11 +7796,11 @@
       <c r="H148" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I148" s="2" t="s">
-        <v>450</v>
+      <c r="I148" t="s">
+        <v>674</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>554</v>
@@ -7886,11 +7831,11 @@
       <c r="H149" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I149" s="2" t="s">
-        <v>453</v>
+      <c r="I149" t="s">
+        <v>674</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K149" s="2" t="s">
         <v>554</v>
@@ -7921,11 +7866,11 @@
       <c r="H150" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I150" s="2" t="s">
-        <v>456</v>
+      <c r="I150" t="s">
+        <v>674</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K150" s="2" t="s">
         <v>554</v>
@@ -7956,11 +7901,11 @@
       <c r="H151" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I151" s="2" t="s">
-        <v>459</v>
+      <c r="I151" t="s">
+        <v>674</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K151" s="2" t="s">
         <v>554</v>
@@ -7991,11 +7936,11 @@
       <c r="H152" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I152" s="2" t="s">
-        <v>462</v>
+      <c r="I152" t="s">
+        <v>674</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K152" s="2" t="s">
         <v>554</v>
@@ -8026,11 +7971,11 @@
       <c r="H153" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I153" s="2" t="s">
-        <v>626</v>
+      <c r="I153" t="s">
+        <v>673</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K153" s="2" t="s">
         <v>554</v>
@@ -8061,11 +8006,11 @@
       <c r="H154" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I154" s="2" t="s">
-        <v>626</v>
+      <c r="I154" t="s">
+        <v>673</v>
       </c>
       <c r="J154" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K154" s="2" t="s">
         <v>554</v>
@@ -8096,11 +8041,11 @@
       <c r="H155" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I155" s="2" t="s">
-        <v>471</v>
+      <c r="I155" t="s">
+        <v>674</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K155" s="2" t="s">
         <v>554</v>
@@ -8131,11 +8076,11 @@
       <c r="H156" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I156" s="2" t="s">
-        <v>474</v>
+      <c r="I156" t="s">
+        <v>673</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K156" s="2" t="s">
         <v>554</v>
@@ -8166,11 +8111,11 @@
       <c r="H157" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I157" s="2" t="s">
-        <v>477</v>
+      <c r="I157" t="s">
+        <v>674</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>628</v>
+        <v>606</v>
       </c>
       <c r="K157" s="2" t="s">
         <v>554</v>
@@ -8201,11 +8146,11 @@
       <c r="H158" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I158" s="2" t="s">
-        <v>480</v>
+      <c r="I158" t="s">
+        <v>674</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K158" s="2" t="s">
         <v>554</v>
@@ -8236,11 +8181,11 @@
       <c r="H159" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I159" s="2" t="s">
-        <v>483</v>
+      <c r="I159" t="s">
+        <v>674</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K159" s="2" t="s">
         <v>554</v>
@@ -8271,11 +8216,11 @@
       <c r="H160" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I160" s="2" t="s">
-        <v>486</v>
+      <c r="I160" t="s">
+        <v>674</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K160" s="2" t="s">
         <v>554</v>
@@ -8306,11 +8251,11 @@
       <c r="H161" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I161" s="2" t="s">
-        <v>489</v>
+      <c r="I161" t="s">
+        <v>674</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K161" s="2" t="s">
         <v>554</v>
@@ -8341,11 +8286,11 @@
       <c r="H162" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I162" s="2" t="s">
-        <v>492</v>
+      <c r="I162" t="s">
+        <v>674</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>554</v>
@@ -8376,11 +8321,11 @@
       <c r="H163" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I163" s="2" t="s">
-        <v>495</v>
+      <c r="I163" t="s">
+        <v>674</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K163" s="2" t="s">
         <v>554</v>
@@ -8411,11 +8356,11 @@
       <c r="H164" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I164" s="2" t="s">
-        <v>498</v>
+      <c r="I164" t="s">
+        <v>673</v>
       </c>
       <c r="J164" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K164" s="2" t="s">
         <v>554</v>
@@ -8446,11 +8391,11 @@
       <c r="H165" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I165" s="2" t="s">
-        <v>501</v>
+      <c r="I165" t="s">
+        <v>673</v>
       </c>
       <c r="J165" s="2" t="s">
-        <v>629</v>
+        <v>607</v>
       </c>
       <c r="K165" s="2" t="s">
         <v>554</v>
@@ -8481,11 +8426,11 @@
       <c r="H166" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I166" s="2" t="s">
-        <v>626</v>
+      <c r="I166" t="s">
+        <v>673</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>554</v>
@@ -8516,14 +8461,14 @@
       <c r="H167" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I167" s="2" t="s">
-        <v>507</v>
+      <c r="I167" t="s">
+        <v>552</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K167" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
@@ -8551,14 +8496,14 @@
       <c r="H168" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I168" s="2" t="s">
-        <v>510</v>
+      <c r="I168" t="s">
+        <v>552</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
@@ -8586,11 +8531,11 @@
       <c r="H169" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I169" s="2" t="s">
-        <v>513</v>
+      <c r="I169" t="s">
+        <v>673</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K169" s="2" t="s">
         <v>554</v>
@@ -8621,11 +8566,11 @@
       <c r="H170" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I170" s="2" t="s">
-        <v>516</v>
+      <c r="I170" t="s">
+        <v>674</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K170" s="2" t="s">
         <v>554</v>
@@ -8656,14 +8601,14 @@
       <c r="H171" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I171" s="2" t="s">
-        <v>519</v>
+      <c r="I171" t="s">
+        <v>552</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="K171" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
@@ -8691,14 +8636,14 @@
       <c r="H172" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I172" s="2" t="s">
-        <v>522</v>
+      <c r="I172" t="s">
+        <v>552</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
@@ -8726,14 +8671,14 @@
       <c r="H173" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I173" s="2" t="s">
-        <v>525</v>
+      <c r="I173" t="s">
+        <v>552</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K173" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
@@ -8761,11 +8706,11 @@
       <c r="H174" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I174" s="2" t="s">
-        <v>528</v>
+      <c r="I174" t="s">
+        <v>674</v>
       </c>
       <c r="J174" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K174" s="2" t="s">
         <v>554</v>
@@ -8796,11 +8741,11 @@
       <c r="H175" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I175" s="2" t="s">
-        <v>531</v>
+      <c r="I175" t="s">
+        <v>674</v>
       </c>
       <c r="J175" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="K175" s="2" t="s">
         <v>554</v>
@@ -8831,11 +8776,11 @@
       <c r="H176" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I176" s="2" t="s">
-        <v>631</v>
+      <c r="I176" t="s">
+        <v>673</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K176" s="2" t="s">
         <v>554</v>
@@ -8866,11 +8811,11 @@
       <c r="H177" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I177" s="2" t="s">
-        <v>537</v>
+      <c r="I177" t="s">
+        <v>552</v>
       </c>
       <c r="J177" s="2" t="s">
-        <v>632</v>
+        <v>609</v>
       </c>
       <c r="K177" s="2" t="s">
         <v>535</v>
@@ -8901,14 +8846,14 @@
       <c r="H178" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I178" s="2" t="s">
-        <v>633</v>
+      <c r="I178" t="s">
+        <v>552</v>
       </c>
       <c r="J178" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K178" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
@@ -8936,14 +8881,14 @@
       <c r="H179" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I179" s="2" t="s">
-        <v>633</v>
+      <c r="I179" t="s">
+        <v>552</v>
       </c>
       <c r="J179" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K179" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
@@ -8971,11 +8916,11 @@
       <c r="H180" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I180" s="2" t="s">
-        <v>546</v>
+      <c r="I180" t="s">
+        <v>673</v>
       </c>
       <c r="J180" s="2" t="s">
-        <v>634</v>
+        <v>610</v>
       </c>
       <c r="K180" s="2" t="s">
         <v>554</v>
@@ -9006,49 +8951,49 @@
       <c r="H181" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I181" s="2" t="s">
-        <v>633</v>
+      <c r="I181" t="s">
+        <v>552</v>
       </c>
       <c r="J181" s="2" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="K181" s="2" t="s">
-        <v>688</v>
+        <v>663</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
-        <v>638</v>
+        <v>613</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>639</v>
+        <v>614</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>640</v>
+        <v>615</v>
       </c>
       <c r="D182" s="2">
         <v>0</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>642</v>
+        <v>617</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>643</v>
+        <v>618</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="I182" s="2" t="s">
-        <v>640</v>
+        <v>616</v>
+      </c>
+      <c r="I182" t="s">
+        <v>613</v>
       </c>
       <c r="J182" s="2" t="s">
-        <v>640</v>
+        <v>615</v>
       </c>
       <c r="K182" s="2" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -9060,7 +9005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34021EF-588F-42F2-AB27-A495691385C8}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -9391,7 +9336,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>697</v>
+        <v>672</v>
       </c>
       <c r="B7" s="9">
         <v>83</v>
@@ -9581,7 +9526,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>658</v>
+        <v>633</v>
       </c>
       <c r="B2" s="9">
         <v>74</v>
@@ -9595,7 +9540,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>659</v>
+        <v>634</v>
       </c>
       <c r="B3" s="9">
         <v>75</v>
@@ -9609,7 +9554,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>660</v>
+        <v>635</v>
       </c>
       <c r="B4" s="9">
         <v>76</v>
@@ -9884,21 +9829,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>651</v>
+        <v>626</v>
       </c>
       <c r="B1" t="s">
-        <v>649</v>
+        <v>624</v>
       </c>
       <c r="C1" t="s">
-        <v>650</v>
+        <v>625</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="B2" t="s">
-        <v>644</v>
+        <v>619</v>
       </c>
       <c r="C2">
         <v>5622</v>
@@ -9906,10 +9851,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>656</v>
+        <v>631</v>
       </c>
       <c r="B3" t="s">
-        <v>645</v>
+        <v>620</v>
       </c>
       <c r="C3">
         <v>5922</v>
@@ -9917,10 +9862,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>654</v>
+        <v>629</v>
       </c>
       <c r="B4" t="s">
-        <v>646</v>
+        <v>621</v>
       </c>
       <c r="C4">
         <v>5516</v>
@@ -9928,10 +9873,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>652</v>
+        <v>627</v>
       </c>
       <c r="B5" t="s">
-        <v>647</v>
+        <v>622</v>
       </c>
       <c r="C5">
         <v>5616</v>
@@ -9939,10 +9884,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>653</v>
+        <v>628</v>
       </c>
       <c r="B6" t="s">
-        <v>648</v>
+        <v>623</v>
       </c>
       <c r="C6">
         <v>5916</v>
@@ -9950,10 +9895,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>657</v>
+        <v>632</v>
       </c>
       <c r="B7" t="s">
-        <v>646</v>
+        <v>621</v>
       </c>
       <c r="C7">
         <v>5516</v>
@@ -10490,36 +10435,36 @@
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>661</v>
+        <v>636</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>662</v>
+        <v>637</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>663</v>
+        <v>638</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>664</v>
+        <v>639</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>665</v>
+        <v>640</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>666</v>
+        <v>641</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>667</v>
+        <v>642</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B2" s="18">
         <v>78</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>695</v>
+        <v>670</v>
       </c>
       <c r="D2" s="14">
         <v>0</v>
@@ -10536,13 +10481,13 @@
     </row>
     <row r="3" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B3" s="18">
         <v>79</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>696</v>
+        <v>671</v>
       </c>
       <c r="D3" s="14">
         <v>1</v>
@@ -10559,7 +10504,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B4" s="15">
         <v>80</v>
@@ -10582,13 +10527,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B5" s="15">
         <v>81</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>669</v>
+        <v>644</v>
       </c>
       <c r="D5" s="14">
         <v>0</v>
@@ -10605,13 +10550,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B6" s="15">
         <v>82</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>670</v>
+        <v>645</v>
       </c>
       <c r="D6" s="14">
         <v>1</v>
@@ -10628,7 +10573,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B7" s="15">
         <v>83</v>
@@ -10651,13 +10596,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B8" s="15">
         <v>84</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>671</v>
+        <v>646</v>
       </c>
       <c r="D8" s="14">
         <v>1</v>
@@ -10674,13 +10619,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B9" s="15">
         <v>85</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>672</v>
+        <v>647</v>
       </c>
       <c r="D9" s="14">
         <v>1</v>
@@ -10697,13 +10642,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B10" s="15">
         <v>86</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>673</v>
+        <v>648</v>
       </c>
       <c r="D10" s="14">
         <v>1</v>
@@ -10720,13 +10665,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B11" s="15">
         <v>87</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>674</v>
+        <v>649</v>
       </c>
       <c r="D11" s="14">
         <v>0</v>
@@ -10743,13 +10688,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B12" s="15">
         <v>88</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>675</v>
+        <v>650</v>
       </c>
       <c r="D12" s="14">
         <v>0</v>
@@ -10766,13 +10711,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B13" s="15">
         <v>89</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>676</v>
+        <v>651</v>
       </c>
       <c r="D13" s="14">
         <v>0</v>
@@ -10789,13 +10734,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B14" s="15">
         <v>90</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>677</v>
+        <v>652</v>
       </c>
       <c r="D14" s="14">
         <v>0</v>
@@ -10812,7 +10757,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B15" s="15">
         <v>91</v>
@@ -10835,13 +10780,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B16" s="15">
         <v>92</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>678</v>
+        <v>653</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
@@ -10858,13 +10803,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="B17" s="15">
         <v>93</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>679</v>
+        <v>654</v>
       </c>
       <c r="D17" s="14">
         <v>1</v>
@@ -10881,27 +10826,27 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>680</v>
+        <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>681</v>
+        <v>656</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>682</v>
+        <v>657</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>683</v>
+        <v>658</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>684</v>
+        <v>659</v>
       </c>
     </row>
   </sheetData>
@@ -10911,6 +10856,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -10960,7 +10914,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085AB43357A52934F9DA0AE100FA94E83" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e48e03f48db7acc8887685b5226d49bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad97c0c9-42e6-4652-88dc-465719a91e8a" xmlns:ns3="b9517679-4569-40b2-8c6c-5d499fa2fe5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd4da19bcd51d0758a9bab27ec3ba1c9" ns2:_="" ns3:_="">
     <xsd:import namespace="ad97c0c9-42e6-4652-88dc-465719a91e8a"/>
@@ -11216,16 +11170,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6605457E-D50E-4975-B2F5-0EC43ECE5941}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9A2DB72-A0DA-4D68-92F8-17DB9850571B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -11233,7 +11186,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D04D863-F4C5-413F-BEB0-944BBDE9B782}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11250,12 +11203,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6605457E-D50E-4975-B2F5-0EC43ECE5941}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>